<commit_message>
updated version of dataset
</commit_message>
<xml_diff>
--- a/dataset/data_points_indexes.xlsx
+++ b/dataset/data_points_indexes.xlsx
@@ -1,35 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POLYTECH_2025\health_index\dataset\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52FA848-95B6-43E0-AD22-F6E1129D179C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="121">
   <si>
     <t>Кердо</t>
   </si>
@@ -369,377 +362,72 @@
   <si>
     <t>1.5-норма</t>
   </si>
+  <si>
+    <t>….</t>
+  </si>
+  <si>
+    <t>x1*</t>
+  </si>
+  <si>
+    <t>x2*</t>
+  </si>
+  <si>
+    <t>…..</t>
+  </si>
+  <si>
+    <t>x46*</t>
+  </si>
+  <si>
+    <t>index2</t>
+  </si>
+  <si>
+    <t>index3</t>
+  </si>
+  <si>
+    <t>index1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -762,324 +450,42 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1329,24 +735,24 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BY1" workbookViewId="0">
-      <selection activeCell="BY1" sqref="BY1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="93" width="9" style="1"/>
-    <col min="94" max="94" width="17.75" style="1" customWidth="1"/>
-    <col min="95" max="95" width="15.375" style="1" customWidth="1"/>
-    <col min="96" max="96" width="35.25" style="1" customWidth="1"/>
+    <col min="94" max="94" width="17.7109375" style="1" customWidth="1"/>
+    <col min="95" max="95" width="15.42578125" style="1" customWidth="1"/>
+    <col min="96" max="96" width="35.28515625" style="1" customWidth="1"/>
     <col min="97" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1638,12 +1044,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="27" customHeight="1" spans="1:96">
+    <row r="2" spans="1:96" ht="27" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C2" s="3">
         <v>74</v>
@@ -1918,7 +1324,7 @@
       <c r="CO2" s="3">
         <v>78</v>
       </c>
-      <c r="CP2" s="4" t="s">
+      <c r="CP2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="CQ2" s="4" t="s">
@@ -1928,12 +1334,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="26" customHeight="1" spans="1:96">
+    <row r="3" spans="1:96" ht="26.1" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C3" s="3">
         <v>76</v>
@@ -1975,7 +1381,7 @@
         <v>70</v>
       </c>
       <c r="P3" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q3" s="3">
         <v>76</v>
@@ -2077,7 +1483,7 @@
         <v>86</v>
       </c>
       <c r="AX3" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AY3" s="3">
         <v>80</v>
@@ -2113,7 +1519,7 @@
         <v>70</v>
       </c>
       <c r="BJ3" s="3">
-        <v>1.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="BK3" s="3">
         <v>84</v>
@@ -2125,7 +1531,7 @@
         <v>80</v>
       </c>
       <c r="BN3" s="3">
-        <v>1.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="BO3" s="3">
         <v>86</v>
@@ -2155,7 +1561,7 @@
         <v>86</v>
       </c>
       <c r="BX3" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BY3" s="3">
         <v>78</v>
@@ -2208,7 +1614,7 @@
       <c r="CO3" s="3">
         <v>80</v>
       </c>
-      <c r="CP3" s="4" t="s">
+      <c r="CP3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="CQ3" s="4" t="s">
@@ -2218,7 +1624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="24" customHeight="1" spans="1:96">
+    <row r="4" spans="1:96" ht="24" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2301,7 +1707,7 @@
         <v>76</v>
       </c>
       <c r="AB4" s="3">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC4" s="3">
         <v>82</v>
@@ -2319,7 +1725,7 @@
         <v>82</v>
       </c>
       <c r="AH4" s="3">
-        <v>0.07</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="AI4" s="3">
         <v>30</v>
@@ -2349,7 +1755,7 @@
         <v>78</v>
       </c>
       <c r="AR4" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AS4" s="3">
         <v>80</v>
@@ -2391,7 +1797,7 @@
         <v>84</v>
       </c>
       <c r="BF4" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BG4" s="3">
         <v>80</v>
@@ -2439,7 +1845,7 @@
         <v>70</v>
       </c>
       <c r="BV4" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BW4" s="3">
         <v>74</v>
@@ -2451,13 +1857,13 @@
         <v>70</v>
       </c>
       <c r="BZ4" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="CA4" s="3">
         <v>84</v>
       </c>
       <c r="CB4" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="CC4" s="3">
         <v>72</v>
@@ -2508,7 +1914,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" ht="25" customHeight="1" spans="1:96">
+    <row r="5" spans="1:96" ht="24.95" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -2798,12 +2204,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" ht="27" customHeight="1" spans="1:96">
+    <row r="6" spans="1:96" ht="27" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C6" s="3">
         <v>74</v>
@@ -2857,7 +2263,7 @@
         <v>80</v>
       </c>
       <c r="T6" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="U6" s="3">
         <v>84</v>
@@ -2869,7 +2275,7 @@
         <v>80</v>
       </c>
       <c r="X6" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Y6" s="3">
         <v>80</v>
@@ -3088,7 +2494,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" ht="27" customHeight="1" spans="1:96">
+    <row r="7" spans="1:96" ht="27" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -3147,7 +2553,7 @@
         <v>84</v>
       </c>
       <c r="T7" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="U7" s="3">
         <v>82</v>
@@ -3165,7 +2571,7 @@
         <v>88</v>
       </c>
       <c r="Z7" s="3">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="AA7" s="3">
         <v>78</v>
@@ -3201,7 +2607,7 @@
         <v>65</v>
       </c>
       <c r="AL7" s="3">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AM7" s="3">
         <v>76</v>
@@ -3315,7 +2721,7 @@
         <v>66</v>
       </c>
       <c r="BX7" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BY7" s="3">
         <v>80</v>
@@ -3372,13 +2778,13 @@
         <v>21</v>
       </c>
       <c r="CQ7" s="4">
-        <v>70.4</v>
+        <v>70.400000000000006</v>
       </c>
       <c r="CR7" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" ht="27" customHeight="1" spans="1:96">
+    <row r="8" spans="1:96" ht="27" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -3455,7 +2861,7 @@
         <v>80</v>
       </c>
       <c r="Z8" s="3">
-        <v>1.16</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="AA8" s="3">
         <v>60</v>
@@ -3497,13 +2903,13 @@
         <v>80</v>
       </c>
       <c r="AN8" s="3">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AO8" s="3">
         <v>80</v>
       </c>
       <c r="AP8" s="3">
-        <v>1.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="AQ8" s="3">
         <v>66</v>
@@ -3515,7 +2921,7 @@
         <v>88</v>
       </c>
       <c r="AT8" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AU8" s="3">
         <v>64</v>
@@ -3563,13 +2969,13 @@
         <v>72</v>
       </c>
       <c r="BJ8" s="3">
-        <v>1.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="BK8" s="3">
         <v>86</v>
       </c>
       <c r="BL8" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BM8" s="3">
         <v>84</v>
@@ -3599,7 +3005,7 @@
         <v>70</v>
       </c>
       <c r="BV8" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="BW8" s="3">
         <v>70</v>
@@ -3611,13 +3017,13 @@
         <v>70</v>
       </c>
       <c r="BZ8" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="CA8" s="3">
         <v>70</v>
       </c>
       <c r="CB8" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="CC8" s="3">
         <v>80</v>
@@ -3668,7 +3074,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" ht="30" customHeight="1" spans="1:96">
+    <row r="9" spans="1:96" ht="30" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -3757,7 +3163,7 @@
         <v>70</v>
       </c>
       <c r="AD9" s="3">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE9" s="3">
         <v>90</v>
@@ -3895,7 +3301,7 @@
         <v>64</v>
       </c>
       <c r="BX9" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BY9" s="3">
         <v>68</v>
@@ -3958,7 +3364,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" ht="31" customHeight="1" spans="1:96">
+    <row r="10" spans="1:96" ht="30.95" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
@@ -4011,7 +3417,7 @@
         <v>78</v>
       </c>
       <c r="R10" s="3">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S10" s="3">
         <v>76</v>
@@ -4053,7 +3459,7 @@
         <v>80</v>
       </c>
       <c r="AF10" s="3">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AG10" s="3">
         <v>68</v>
@@ -4101,7 +3507,7 @@
         <v>80</v>
       </c>
       <c r="AV10" s="3">
-        <v>0.57</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="AW10" s="3">
         <v>86</v>
@@ -4197,7 +3603,7 @@
         <v>84</v>
       </c>
       <c r="CB10" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="CC10" s="3">
         <v>66</v>
@@ -4248,7 +3654,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" ht="30" customHeight="1" spans="1:96">
+    <row r="11" spans="1:96" ht="30" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
@@ -4271,7 +3677,7 @@
         <v>86</v>
       </c>
       <c r="H11" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I11" s="3">
         <v>94</v>
@@ -4295,7 +3701,7 @@
         <v>90</v>
       </c>
       <c r="P11" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q11" s="3">
         <v>82</v>
@@ -4409,7 +3815,7 @@
         <v>60</v>
       </c>
       <c r="BB11" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BC11" s="3">
         <v>70</v>
@@ -4445,7 +3851,7 @@
         <v>78</v>
       </c>
       <c r="BN11" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BO11" s="3">
         <v>70</v>
@@ -4463,19 +3869,19 @@
         <v>80</v>
       </c>
       <c r="BT11" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BU11" s="3">
         <v>70</v>
       </c>
       <c r="BV11" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BW11" s="3">
         <v>70</v>
       </c>
       <c r="BX11" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BY11" s="3">
         <v>70</v>
@@ -4511,7 +3917,7 @@
         <v>84</v>
       </c>
       <c r="CJ11" s="3">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="CK11" s="3">
         <v>80</v>
@@ -4538,7 +3944,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" ht="33" customHeight="1" spans="1:96">
+    <row r="12" spans="1:96" ht="33" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>34</v>
       </c>
@@ -4579,19 +3985,19 @@
         <v>78</v>
       </c>
       <c r="N12" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="O12" s="3">
         <v>86</v>
       </c>
       <c r="P12" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="Q12" s="3">
         <v>78</v>
       </c>
       <c r="R12" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="S12" s="3">
         <v>76</v>
@@ -4627,7 +4033,7 @@
         <v>87</v>
       </c>
       <c r="AD12" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AE12" s="3">
         <v>78</v>
@@ -4675,7 +4081,7 @@
         <v>78</v>
       </c>
       <c r="AT12" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AU12" s="3">
         <v>76</v>
@@ -4765,7 +4171,7 @@
         <v>58</v>
       </c>
       <c r="BX12" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BY12" s="3">
         <v>60</v>
@@ -4828,12 +4234,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" ht="30" customHeight="1" spans="1:96">
+    <row r="13" spans="1:96" ht="30" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C13" s="3">
         <v>90</v>
@@ -4947,13 +4353,13 @@
         <v>70</v>
       </c>
       <c r="AN13" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AO13" s="3">
         <v>88</v>
       </c>
       <c r="AP13" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AQ13" s="3">
         <v>86</v>
@@ -5049,7 +4455,7 @@
         <v>70</v>
       </c>
       <c r="BV13" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BW13" s="3">
         <v>70</v>
@@ -5112,13 +4518,13 @@
         <v>38</v>
       </c>
       <c r="CQ13" s="4">
-        <v>76.43</v>
+        <v>76.430000000000007</v>
       </c>
       <c r="CR13" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" ht="45" spans="1:96">
+    <row r="14" spans="1:96">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -5129,7 +4535,7 @@
         <v>66</v>
       </c>
       <c r="D14" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E14" s="3">
         <v>81</v>
@@ -5141,7 +4547,7 @@
         <v>70</v>
       </c>
       <c r="H14" s="3">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I14" s="3">
         <v>64</v>
@@ -5177,19 +4583,19 @@
         <v>68</v>
       </c>
       <c r="T14" s="3">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="U14" s="3">
         <v>66</v>
       </c>
       <c r="V14" s="3">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="W14" s="3">
         <v>70</v>
       </c>
       <c r="X14" s="3">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="Y14" s="3">
         <v>66</v>
@@ -5303,7 +4709,7 @@
         <v>78</v>
       </c>
       <c r="BJ14" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BK14" s="3">
         <v>68</v>
@@ -5408,7 +4814,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" ht="31" customHeight="1" spans="1:96">
+    <row r="15" spans="1:96" ht="30.95" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -5491,7 +4897,7 @@
         <v>78</v>
       </c>
       <c r="AB15" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AC15" s="3">
         <v>82</v>
@@ -5503,7 +4909,7 @@
         <v>66</v>
       </c>
       <c r="AF15" s="3">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AG15" s="3">
         <v>76</v>
@@ -5539,13 +4945,13 @@
         <v>80</v>
       </c>
       <c r="AR15" s="3">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AS15" s="3">
         <v>88</v>
       </c>
       <c r="AT15" s="3">
-        <v>0.58</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="AU15" s="3">
         <v>80</v>
@@ -5617,7 +5023,7 @@
         <v>80</v>
       </c>
       <c r="BR15" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BS15" s="3">
         <v>84</v>
@@ -5659,7 +5065,7 @@
         <v>86</v>
       </c>
       <c r="CF15" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="CG15" s="3">
         <v>90</v>
@@ -5698,7 +5104,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" ht="35" customHeight="1" spans="1:96">
+    <row r="16" spans="1:96" ht="35.1" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>46</v>
       </c>
@@ -5781,7 +5187,7 @@
         <v>80</v>
       </c>
       <c r="AB16" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AC16" s="3">
         <v>82</v>
@@ -5823,7 +5229,7 @@
         <v>76</v>
       </c>
       <c r="AP16" s="3">
-        <v>1.16</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="AQ16" s="3">
         <v>76</v>
@@ -5835,7 +5241,7 @@
         <v>70</v>
       </c>
       <c r="AT16" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AU16" s="3">
         <v>78</v>
@@ -5895,7 +5301,7 @@
         <v>60</v>
       </c>
       <c r="BN16" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BO16" s="3">
         <v>66</v>
@@ -5913,7 +5319,7 @@
         <v>70</v>
       </c>
       <c r="BT16" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BU16" s="3">
         <v>52</v>
@@ -5988,7 +5394,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" ht="45" spans="1:96">
+    <row r="17" spans="1:96">
       <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
@@ -6065,7 +5471,7 @@
         <v>86</v>
       </c>
       <c r="Z17" s="3">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA17" s="3">
         <v>88</v>
@@ -6149,7 +5555,7 @@
         <v>60</v>
       </c>
       <c r="BB17" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BC17" s="3">
         <v>68</v>
@@ -6197,7 +5603,7 @@
         <v>62</v>
       </c>
       <c r="BR17" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BS17" s="3">
         <v>70</v>
@@ -6215,7 +5621,7 @@
         <v>84</v>
       </c>
       <c r="BX17" s="3">
-        <v>1.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="BY17" s="3">
         <v>74</v>
@@ -6278,7 +5684,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" ht="45" spans="1:96">
+    <row r="18" spans="1:96">
       <c r="A18" s="3" t="s">
         <v>52</v>
       </c>
@@ -6313,7 +5719,7 @@
         <v>84</v>
       </c>
       <c r="L18" s="3">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M18" s="3">
         <v>72</v>
@@ -6493,7 +5899,7 @@
         <v>64</v>
       </c>
       <c r="BT18" s="3">
-        <v>1.16</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="BU18" s="3">
         <v>72</v>
@@ -6568,7 +5974,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" ht="45" spans="1:96">
+    <row r="19" spans="1:96">
       <c r="A19" s="3" t="s">
         <v>55</v>
       </c>
@@ -6858,7 +6264,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" ht="45" spans="1:96">
+    <row r="20" spans="1:96">
       <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
@@ -6875,7 +6281,7 @@
         <v>82</v>
       </c>
       <c r="F20" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G20" s="3">
         <v>84</v>
@@ -6893,7 +6299,7 @@
         <v>80</v>
       </c>
       <c r="L20" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M20" s="3">
         <v>86</v>
@@ -6905,7 +6311,7 @@
         <v>88</v>
       </c>
       <c r="P20" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q20" s="3">
         <v>80</v>
@@ -6983,13 +6389,13 @@
         <v>86</v>
       </c>
       <c r="AP20" s="3">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AQ20" s="3">
         <v>84</v>
       </c>
       <c r="AR20" s="3">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AS20" s="3">
         <v>80</v>
@@ -7148,7 +6554,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" ht="45" spans="1:96">
+    <row r="21" spans="1:96">
       <c r="A21" s="3" t="s">
         <v>60</v>
       </c>
@@ -7159,7 +6565,7 @@
         <v>72</v>
       </c>
       <c r="D21" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E21" s="3">
         <v>74</v>
@@ -7381,13 +6787,13 @@
         <v>70</v>
       </c>
       <c r="BZ21" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="CA21" s="3">
         <v>74</v>
       </c>
       <c r="CB21" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="CC21" s="3">
         <v>70</v>
@@ -7438,7 +6844,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" ht="45" spans="1:96">
+    <row r="22" spans="1:96">
       <c r="A22" s="3" t="s">
         <v>63</v>
       </c>
@@ -7491,7 +6897,7 @@
         <v>20</v>
       </c>
       <c r="R22" s="3">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S22" s="3">
         <v>90</v>
@@ -7647,7 +7053,7 @@
         <v>70</v>
       </c>
       <c r="BR22" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BS22" s="3">
         <v>60</v>
@@ -7659,7 +7065,7 @@
         <v>70</v>
       </c>
       <c r="BV22" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BW22" s="3">
         <v>66</v>
@@ -7728,7 +7134,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" ht="37" customHeight="1" spans="1:96">
+    <row r="23" spans="1:96" ht="36.950000000000003" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>66</v>
       </c>
@@ -7751,7 +7157,7 @@
         <v>88</v>
       </c>
       <c r="H23" s="3">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I23" s="3">
         <v>80</v>
@@ -7787,7 +7193,7 @@
         <v>80</v>
       </c>
       <c r="T23" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="U23" s="3">
         <v>76</v>
@@ -7805,7 +7211,7 @@
         <v>82</v>
       </c>
       <c r="Z23" s="3">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AA23" s="3">
         <v>82</v>
@@ -8018,7 +7424,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" ht="36" customHeight="1" spans="1:96">
+    <row r="24" spans="1:96" ht="36" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>69</v>
       </c>
@@ -8053,7 +7459,7 @@
         <v>84</v>
       </c>
       <c r="L24" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M24" s="3">
         <v>88</v>
@@ -8107,13 +7513,13 @@
         <v>86</v>
       </c>
       <c r="AD24" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="AE24" s="3">
         <v>80</v>
       </c>
       <c r="AF24" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AG24" s="3">
         <v>74</v>
@@ -8137,7 +7543,7 @@
         <v>76</v>
       </c>
       <c r="AN24" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="AO24" s="3">
         <v>74</v>
@@ -8155,19 +7561,19 @@
         <v>78</v>
       </c>
       <c r="AT24" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="AU24" s="3">
         <v>78</v>
       </c>
       <c r="AV24" s="3">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="AW24" s="3">
         <v>76</v>
       </c>
       <c r="AX24" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AY24" s="3">
         <v>70</v>
@@ -8191,13 +7597,13 @@
         <v>70</v>
       </c>
       <c r="BF24" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BG24" s="3">
         <v>78</v>
       </c>
       <c r="BH24" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="BI24" s="3">
         <v>68</v>
@@ -8215,7 +7621,7 @@
         <v>74</v>
       </c>
       <c r="BN24" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BO24" s="3">
         <v>68</v>
@@ -8239,7 +7645,7 @@
         <v>84</v>
       </c>
       <c r="BV24" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="BW24" s="3">
         <v>76</v>
@@ -8281,7 +7687,7 @@
         <v>80</v>
       </c>
       <c r="CJ24" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="CK24" s="3">
         <v>78</v>
@@ -8308,7 +7714,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" ht="45" spans="1:96">
+    <row r="25" spans="1:96">
       <c r="A25" s="3" t="s">
         <v>71</v>
       </c>
@@ -8319,13 +7725,13 @@
         <v>72</v>
       </c>
       <c r="D25" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E25" s="3">
         <v>66</v>
       </c>
       <c r="F25" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G25" s="3">
         <v>66</v>
@@ -8373,7 +7779,7 @@
         <v>74</v>
       </c>
       <c r="V25" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="W25" s="3">
         <v>76</v>
@@ -8445,13 +7851,13 @@
         <v>70</v>
       </c>
       <c r="AT25" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="AU25" s="3">
         <v>72</v>
       </c>
       <c r="AV25" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AW25" s="3">
         <v>70</v>
@@ -8592,13 +7998,13 @@
         <v>72</v>
       </c>
       <c r="CQ25" s="4">
-        <v>69.43</v>
+        <v>69.430000000000007</v>
       </c>
       <c r="CR25" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" ht="39" customHeight="1" spans="1:96">
+    <row r="26" spans="1:96" ht="39" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>74</v>
       </c>
@@ -8621,7 +8027,7 @@
         <v>76</v>
       </c>
       <c r="H26" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I26" s="3">
         <v>88</v>
@@ -8645,7 +8051,7 @@
         <v>90</v>
       </c>
       <c r="P26" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q26" s="3">
         <v>84</v>
@@ -8765,7 +8171,7 @@
         <v>76</v>
       </c>
       <c r="BD26" s="3">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="BE26" s="3">
         <v>66</v>
@@ -8813,7 +8219,7 @@
         <v>66</v>
       </c>
       <c r="BT26" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BU26" s="3">
         <v>74</v>
@@ -8849,7 +8255,7 @@
         <v>98</v>
       </c>
       <c r="CF26" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="CG26" s="3">
         <v>90</v>
@@ -8888,7 +8294,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" ht="37" customHeight="1" spans="1:96">
+    <row r="27" spans="1:96" ht="36.950000000000003" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>77</v>
       </c>
@@ -8941,7 +8347,7 @@
         <v>88</v>
       </c>
       <c r="R27" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="S27" s="3">
         <v>90</v>
@@ -9049,7 +8455,7 @@
         <v>80</v>
       </c>
       <c r="BB27" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BC27" s="3">
         <v>68</v>
@@ -9061,19 +8467,19 @@
         <v>90</v>
       </c>
       <c r="BF27" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BG27" s="3">
         <v>84</v>
       </c>
       <c r="BH27" s="3">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="BI27" s="3">
         <v>70</v>
       </c>
       <c r="BJ27" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BK27" s="3">
         <v>84</v>
@@ -9091,7 +8497,7 @@
         <v>78</v>
       </c>
       <c r="BP27" s="3">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="BQ27" s="3">
         <v>70</v>
@@ -9103,7 +8509,7 @@
         <v>76</v>
       </c>
       <c r="BT27" s="3">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="BU27" s="3">
         <v>86</v>
@@ -9115,7 +8521,7 @@
         <v>78</v>
       </c>
       <c r="BX27" s="3">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="BY27" s="3">
         <v>66</v>
@@ -9127,7 +8533,7 @@
         <v>82</v>
       </c>
       <c r="CB27" s="3">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="CC27" s="3">
         <v>78</v>
@@ -9139,7 +8545,7 @@
         <v>90</v>
       </c>
       <c r="CF27" s="3">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="CG27" s="3">
         <v>90</v>
@@ -9178,12 +8584,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" ht="45" spans="1:96">
+    <row r="28" spans="1:96">
       <c r="A28" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B28" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C28" s="3">
         <v>70</v>
@@ -9219,7 +8625,7 @@
         <v>78</v>
       </c>
       <c r="N28" s="3">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="O28" s="3">
         <v>84</v>
@@ -9243,7 +8649,7 @@
         <v>70</v>
       </c>
       <c r="V28" s="3">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="W28" s="3">
         <v>72</v>
@@ -9267,13 +8673,13 @@
         <v>84</v>
       </c>
       <c r="AD28" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AE28" s="3">
         <v>70</v>
       </c>
       <c r="AF28" s="3">
-        <v>1.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="AG28" s="3">
         <v>80</v>
@@ -9303,7 +8709,7 @@
         <v>78</v>
       </c>
       <c r="AP28" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AQ28" s="3">
         <v>62</v>
@@ -9315,7 +8721,7 @@
         <v>80</v>
       </c>
       <c r="AT28" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AU28" s="3">
         <v>70</v>
@@ -9345,7 +8751,7 @@
         <v>50</v>
       </c>
       <c r="BD28" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BE28" s="3">
         <v>70</v>
@@ -9381,7 +8787,7 @@
         <v>64</v>
       </c>
       <c r="BP28" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BQ28" s="3">
         <v>68</v>
@@ -9417,7 +8823,7 @@
         <v>70</v>
       </c>
       <c r="CB28" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="CC28" s="3">
         <v>60</v>
@@ -9468,7 +8874,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" ht="39" customHeight="1" spans="1:96">
+    <row r="29" spans="1:96" ht="39" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>81</v>
       </c>
@@ -9479,7 +8885,7 @@
         <v>80</v>
       </c>
       <c r="D29" s="3">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E29" s="3">
         <v>80</v>
@@ -9497,7 +8903,7 @@
         <v>86</v>
       </c>
       <c r="J29" s="3">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="K29" s="3">
         <v>80</v>
@@ -9527,7 +8933,7 @@
         <v>74</v>
       </c>
       <c r="T29" s="3">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="U29" s="3">
         <v>70</v>
@@ -9758,7 +9164,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" ht="40" customHeight="1" spans="1:96">
+    <row r="30" spans="1:96" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>83</v>
       </c>
@@ -10009,7 +9415,7 @@
         <v>60</v>
       </c>
       <c r="CF30" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="CG30" s="3">
         <v>64</v>
@@ -10048,7 +9454,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" ht="36" customHeight="1" spans="1:96">
+    <row r="31" spans="1:96" ht="36" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>86</v>
       </c>
@@ -10083,7 +9489,7 @@
         <v>80</v>
       </c>
       <c r="L31" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M31" s="3">
         <v>84</v>
@@ -10107,7 +9513,7 @@
         <v>70</v>
       </c>
       <c r="T31" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="U31" s="3">
         <v>70</v>
@@ -10338,7 +9744,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" ht="45" spans="1:96">
+    <row r="32" spans="1:96">
       <c r="A32" s="3" t="s">
         <v>89</v>
       </c>
@@ -10373,7 +9779,7 @@
         <v>68</v>
       </c>
       <c r="L32" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M32" s="3">
         <v>68</v>
@@ -10427,7 +9833,7 @@
         <v>86</v>
       </c>
       <c r="AD32" s="3">
-        <v>1.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="AE32" s="3">
         <v>74</v>
@@ -10469,7 +9875,7 @@
         <v>60</v>
       </c>
       <c r="AR32" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AS32" s="3">
         <v>60</v>
@@ -10628,7 +10034,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" ht="33" customHeight="1" spans="1:96">
+    <row r="33" spans="1:96" ht="33" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>91</v>
       </c>
@@ -10639,7 +10045,7 @@
         <v>82</v>
       </c>
       <c r="D33" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E33" s="3">
         <v>86</v>
@@ -10918,12 +10324,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" ht="35" customHeight="1" spans="1:96">
+    <row r="34" spans="1:96" ht="35.1" customHeight="1">
       <c r="A34" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B34" s="3">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C34" s="3">
         <v>80</v>
@@ -11073,7 +10479,7 @@
         <v>60</v>
       </c>
       <c r="AZ34" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="BA34" s="3">
         <v>78</v>
@@ -11091,7 +10497,7 @@
         <v>76</v>
       </c>
       <c r="BF34" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BG34" s="3">
         <v>80</v>
@@ -11127,7 +10533,7 @@
         <v>60</v>
       </c>
       <c r="BR34" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BS34" s="3">
         <v>70</v>
@@ -11208,7 +10614,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" ht="45" spans="1:96">
+    <row r="35" spans="1:96">
       <c r="A35" s="3" t="s">
         <v>97</v>
       </c>
@@ -11267,13 +10673,13 @@
         <v>80</v>
       </c>
       <c r="T35" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="U35" s="3">
         <v>80</v>
       </c>
       <c r="V35" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="W35" s="3">
         <v>84</v>
@@ -11309,7 +10715,7 @@
         <v>74</v>
       </c>
       <c r="AH35" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AI35" s="3">
         <v>78</v>
@@ -11327,13 +10733,13 @@
         <v>80</v>
       </c>
       <c r="AN35" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AO35" s="3">
         <v>82</v>
       </c>
       <c r="AP35" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AQ35" s="3">
         <v>74</v>
@@ -11351,7 +10757,7 @@
         <v>76</v>
       </c>
       <c r="AV35" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AW35" s="3">
         <v>82</v>
@@ -11393,7 +10799,7 @@
         <v>64</v>
       </c>
       <c r="BJ35" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BK35" s="3">
         <v>66</v>
@@ -11498,7 +10904,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" ht="39" customHeight="1" spans="1:96">
+    <row r="36" spans="1:96" ht="39" customHeight="1">
       <c r="A36" s="3" t="s">
         <v>99</v>
       </c>
@@ -11623,7 +11029,7 @@
         <v>75</v>
       </c>
       <c r="AP36" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AQ36" s="3">
         <v>80</v>
@@ -11635,7 +11041,7 @@
         <v>70</v>
       </c>
       <c r="AT36" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AU36" s="3">
         <v>66</v>
@@ -11671,7 +11077,7 @@
         <v>62</v>
       </c>
       <c r="BF36" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BG36" s="3">
         <v>50</v>
@@ -11719,7 +11125,7 @@
         <v>70</v>
       </c>
       <c r="BV36" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BW36" s="3">
         <v>58</v>
@@ -11782,13 +11188,13 @@
         <v>100</v>
       </c>
       <c r="CQ36" s="4">
-        <v>80.1</v>
+        <v>80.099999999999994</v>
       </c>
       <c r="CR36" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="37" ht="45" spans="1:96">
+    <row r="37" spans="1:96">
       <c r="A37" s="3" t="s">
         <v>102</v>
       </c>
@@ -11901,13 +11307,13 @@
         <v>72</v>
       </c>
       <c r="AL37" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AM37" s="3">
         <v>66</v>
       </c>
       <c r="AN37" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AO37" s="3">
         <v>80</v>
@@ -11925,7 +11331,7 @@
         <v>70</v>
       </c>
       <c r="AT37" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AU37" s="3">
         <v>84</v>
@@ -11949,7 +11355,7 @@
         <v>34</v>
       </c>
       <c r="BB37" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BC37" s="3">
         <v>46</v>
@@ -12009,7 +11415,7 @@
         <v>60</v>
       </c>
       <c r="BV37" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BW37" s="3">
         <v>62</v>
@@ -12027,7 +11433,7 @@
         <v>68</v>
       </c>
       <c r="CB37" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="CC37" s="3">
         <v>80</v>
@@ -12072,13 +11478,13 @@
         <v>103</v>
       </c>
       <c r="CQ37" s="4">
-        <v>73.01</v>
+        <v>73.010000000000005</v>
       </c>
       <c r="CR37" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="38" ht="36" customHeight="1" spans="1:96">
+    <row r="38" spans="1:96" ht="36" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>105</v>
       </c>
@@ -12143,7 +11549,7 @@
         <v>70</v>
       </c>
       <c r="V38" s="3">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="W38" s="3">
         <v>72</v>
@@ -12368,7 +11774,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" ht="38" customHeight="1" spans="1:96">
+    <row r="39" spans="1:96" ht="38.1" customHeight="1">
       <c r="A39" s="3" t="s">
         <v>107</v>
       </c>
@@ -12475,7 +11881,7 @@
         <v>80</v>
       </c>
       <c r="AJ39" s="3">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AK39" s="3">
         <v>84</v>
@@ -12553,7 +11959,7 @@
         <v>68</v>
       </c>
       <c r="BJ39" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BK39" s="3">
         <v>30</v>
@@ -12595,7 +12001,7 @@
         <v>70</v>
       </c>
       <c r="BX39" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BY39" s="3">
         <v>66</v>
@@ -12619,7 +12025,7 @@
         <v>60</v>
       </c>
       <c r="CF39" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="CG39" s="3">
         <v>74</v>
@@ -12658,7 +12064,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" ht="38" customHeight="1" spans="1:96">
+    <row r="40" spans="1:96" ht="38.1" customHeight="1">
       <c r="A40" s="3" t="s">
         <v>110</v>
       </c>
@@ -12855,7 +12261,7 @@
         <v>54</v>
       </c>
       <c r="BN40" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BO40" s="3">
         <v>66</v>
@@ -12948,7 +12354,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" ht="45" spans="1:96">
+    <row r="41" spans="1:96">
       <c r="A41" s="3" t="s">
         <v>111</v>
       </c>
@@ -12995,7 +12401,7 @@
         <v>96</v>
       </c>
       <c r="P41" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q41" s="3">
         <v>86</v>
@@ -13031,7 +12437,7 @@
         <v>76</v>
       </c>
       <c r="AB41" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AC41" s="3">
         <v>86</v>
@@ -13085,7 +12491,7 @@
         <v>68</v>
       </c>
       <c r="AT41" s="3">
-        <v>0.58</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="AU41" s="3">
         <v>76</v>
@@ -13109,7 +12515,7 @@
         <v>70</v>
       </c>
       <c r="BB41" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BC41" s="3">
         <v>46</v>
@@ -13145,7 +12551,7 @@
         <v>66</v>
       </c>
       <c r="BN41" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BO41" s="3">
         <v>70</v>
@@ -13241,40 +12647,80 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>